<commit_message>
calculated average transition error rate
</commit_message>
<xml_diff>
--- a/analyses/DNR_Skyline_20170524/error-checking/2017-06-10-error-checking.xlsx
+++ b/analyses/DNR_Skyline_20170524/error-checking/2017-06-10-error-checking.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yaaminivenkataraman/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yaaminivenkataraman/Documents/project-oyster-oa/analyses/DNR_Skyline_20170524/error-checking/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="2017-06-10-error-checking" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="225">
   <si>
     <t>protein</t>
   </si>
@@ -699,6 +699,9 @@
   </si>
   <si>
     <t>R.EQGVLDVDTLLLR.R, [182, 194]</t>
+  </si>
+  <si>
+    <t>Average peptide error</t>
   </si>
 </sst>
 </file>
@@ -1053,11 +1056,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y103"/>
+  <dimension ref="A1:AA103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X90" sqref="X90"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <pane ySplit="10" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AA104" sqref="AA104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6744,7 +6747,7 @@
         <v>1</v>
       </c>
       <c r="X72">
-        <f t="shared" ref="X71:X101" si="3">SUM(C72:W72)/21</f>
+        <f t="shared" ref="X72:X101" si="3">SUM(C72:W72)/21</f>
         <v>0.8571428571428571</v>
       </c>
       <c r="Y72">
@@ -8648,7 +8651,7 @@
         <v>0.33333333333333337</v>
       </c>
     </row>
-    <row r="97" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>211</v>
       </c>
@@ -8727,7 +8730,7 @@
         <v>9.5238095238095233E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>213</v>
       </c>
@@ -8806,7 +8809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>215</v>
       </c>
@@ -8885,7 +8888,7 @@
         <v>0.4285714285714286</v>
       </c>
     </row>
-    <row r="100" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>217</v>
       </c>
@@ -8964,7 +8967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>219</v>
       </c>
@@ -9043,7 +9046,7 @@
         <v>0.47619047619047616</v>
       </c>
     </row>
-    <row r="102" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>221</v>
       </c>
@@ -9135,7 +9138,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="103" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>222</v>
       </c>
@@ -9225,6 +9228,13 @@
       <c r="W103">
         <f t="shared" ref="W103" si="26">1-W102</f>
         <v>0.25</v>
+      </c>
+      <c r="Z103" t="s">
+        <v>224</v>
+      </c>
+      <c r="AA103">
+        <f>AVERAGE(Y52:Y101)</f>
+        <v>0.24287218045112785</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
calculated stdev, min, max
</commit_message>
<xml_diff>
--- a/analyses/DNR_Skyline_20170524/error-checking/2017-06-10-error-checking.xlsx
+++ b/analyses/DNR_Skyline_20170524/error-checking/2017-06-10-error-checking.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="228">
   <si>
     <t>protein</t>
   </si>
@@ -702,6 +702,15 @@
   </si>
   <si>
     <t>Average peptide error</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>standard dev</t>
   </si>
 </sst>
 </file>
@@ -1056,11 +1065,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA103"/>
+  <dimension ref="A1:AA105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA104" sqref="AA104"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <pane ySplit="10" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AA106" sqref="AA106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9137,6 +9146,13 @@
         <f t="shared" ref="W102" si="15">SUM(W2:W101)/100</f>
         <v>0.75</v>
       </c>
+      <c r="Z102" t="s">
+        <v>227</v>
+      </c>
+      <c r="AA102">
+        <f>SQRT(_xlfn.VAR.S(Y52:Y101))</f>
+        <v>0.25007966727441827</v>
+      </c>
     </row>
     <row r="103" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
@@ -9235,6 +9251,24 @@
       <c r="AA103">
         <f>AVERAGE(Y52:Y101)</f>
         <v>0.24287218045112785</v>
+      </c>
+    </row>
+    <row r="104" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="Z104" t="s">
+        <v>225</v>
+      </c>
+      <c r="AA104">
+        <f>MIN(Y52:Y101)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="Z105" t="s">
+        <v>226</v>
+      </c>
+      <c r="AA105">
+        <f>MAX(Y53:Y102)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>